<commit_message>
Super Tempo - progress
</commit_message>
<xml_diff>
--- a/SuperTempo/SuperTempo-FC.xlsx
+++ b/SuperTempo/SuperTempo-FC.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-old\SuperTempo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperTempo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2EF063F-CB62-47F6-8582-C7B8F9EC968C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EC2AB6-156E-4F96-9169-226B64471DF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31200" yWindow="2595" windowWidth="15870" windowHeight="11835"/>
+    <workbookView xWindow="41430" yWindow="2730" windowWidth="15870" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="1" r:id="rId1"/>
     <sheet name="V2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="86">
   <si>
     <t>Place</t>
   </si>
@@ -369,11 +369,17 @@
   <si>
     <t>v1</t>
   </si>
+  <si>
+    <t>x = 3423 (hero appears)</t>
+  </si>
+  <si>
+    <t>hero appears</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
@@ -444,11 +450,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading" xfId="1"/>
-    <cellStyle name="Heading1" xfId="2"/>
+    <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Result" xfId="3"/>
-    <cellStyle name="Result2" xfId="4"/>
+    <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -759,10 +765,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N91"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1423,7 +1431,7 @@
         <v>46725</v>
       </c>
       <c r="D44">
-        <f t="shared" ref="D44:D55" si="3">IF(B44="","-",IF(C44="","-",B44-C44))</f>
+        <f t="shared" ref="D44:D58" si="3">IF(B44="","-",IF(C44="","-",B44-C44))</f>
         <v>2435</v>
       </c>
     </row>
@@ -1515,139 +1523,162 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="B51">
-        <v>68394</v>
-      </c>
-      <c r="D51" t="str">
+        <v>63983</v>
+      </c>
+      <c r="C51">
+        <v>59720</v>
+      </c>
+      <c r="D51">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>4263</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="B52">
-        <v>74788</v>
-      </c>
-      <c r="D52" t="str">
+        <v>66173</v>
+      </c>
+      <c r="C52">
+        <v>61804</v>
+      </c>
+      <c r="D52">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>4369</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B53">
-        <v>75923</v>
-      </c>
-      <c r="D53" t="str">
+        <v>68394</v>
+      </c>
+      <c r="C53">
+        <v>64025</v>
+      </c>
+      <c r="D53">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>4369</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="B54">
-        <v>78017</v>
-      </c>
-      <c r="D54" t="str">
+        <v>68825</v>
+      </c>
+      <c r="C54">
+        <v>64455</v>
+      </c>
+      <c r="D54">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="B55">
-        <v>79780</v>
+        <v>74788</v>
       </c>
       <c r="D55" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>75923</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57">
+        <v>78017</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>12</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>79780</v>
       </c>
-      <c r="D57" t="str">
-        <f>IF(B57="","-",IF(C57="","-",B57-C57))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58">
-        <v>81636</v>
-      </c>
       <c r="D58" t="str">
-        <f>IF(B58="","-",IF(C58="","-",B58-C58))</f>
-        <v>-</v>
-      </c>
-      <c r="E58" t="s">
-        <v>57</v>
-      </c>
-      <c r="F58" t="s">
-        <v>58</v>
-      </c>
-      <c r="G58" t="s">
-        <v>59</v>
-      </c>
-      <c r="H58" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59">
-        <v>82955</v>
-      </c>
-      <c r="D59" t="str">
-        <f>IF(B59="","-",IF(C59="","-",B59-C59))</f>
-        <v>-</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B60">
+        <v>79780</v>
+      </c>
+      <c r="D60" t="str">
+        <f>IF(B60="","-",IF(C60="","-",B60-C60))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B61">
+        <v>81636</v>
+      </c>
+      <c r="D61" t="str">
+        <f>IF(B61="","-",IF(C61="","-",B61-C61))</f>
+        <v>-</v>
+      </c>
+      <c r="E61" t="s">
+        <v>57</v>
+      </c>
+      <c r="F61" t="s">
+        <v>58</v>
+      </c>
+      <c r="G61" t="s">
+        <v>59</v>
+      </c>
+      <c r="H61" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
-        <v>86049</v>
+        <v>82955</v>
       </c>
       <c r="D62" t="str">
         <f>IF(B62="","-",IF(C62="","-",B62-C62))</f>
@@ -1656,34 +1687,23 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>63</v>
-      </c>
-      <c r="B63">
-        <v>87616</v>
-      </c>
-      <c r="D63" t="str">
-        <f>IF(B63="","-",IF(C63="","-",B63-C63))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>64</v>
-      </c>
-      <c r="B64">
-        <v>89187</v>
-      </c>
-      <c r="D64" t="str">
-        <f>IF(B64="","-",IF(C64="","-",B64-C64))</f>
-        <v>-</v>
-      </c>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B65">
-        <v>103048</v>
+        <v>86049</v>
       </c>
       <c r="D65" t="str">
         <f>IF(B65="","-",IF(C65="","-",B65-C65))</f>
@@ -1692,30 +1712,34 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B66">
-        <v>106508</v>
+        <v>87616</v>
       </c>
       <c r="D66" t="str">
         <f>IF(B66="","-",IF(C66="","-",B66-C66))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67">
+        <v>89187</v>
+      </c>
+      <c r="D67" t="str">
+        <f>IF(B67="","-",IF(C67="","-",B67-C67))</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68">
-        <v>106508</v>
+        <v>103048</v>
       </c>
       <c r="D68" t="str">
         <f>IF(B68="","-",IF(C68="","-",B68-C68))</f>
@@ -1724,34 +1748,30 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B69">
-        <v>107587</v>
+        <v>106508</v>
       </c>
       <c r="D69" t="str">
         <f>IF(B69="","-",IF(C69="","-",B69-C69))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>68</v>
-      </c>
-      <c r="B70">
-        <v>108015</v>
-      </c>
-      <c r="D70" t="str">
-        <f>IF(B70="","-",IF(C70="","-",B70-C70))</f>
-        <v>-</v>
-      </c>
+    <row r="70" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B71">
-        <v>108724</v>
+        <v>106508</v>
       </c>
       <c r="D71" t="str">
         <f>IF(B71="","-",IF(C71="","-",B71-C71))</f>
@@ -1760,10 +1780,14 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B72">
-        <v>108885</v>
+        <v>107587</v>
+      </c>
+      <c r="D72" t="str">
+        <f>IF(B72="","-",IF(C72="","-",B72-C72))</f>
+        <v>-</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1771,46 +1795,42 @@
         <v>68</v>
       </c>
       <c r="B73">
-        <v>109301</v>
+        <v>108015</v>
       </c>
       <c r="D73" t="str">
-        <f t="shared" ref="D73:D79" si="4">IF(B73="","-",IF(C73="","-",B73-C73))</f>
+        <f>IF(B73="","-",IF(C73="","-",B73-C73))</f>
         <v>-</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B74">
-        <v>109728</v>
+        <v>108724</v>
       </c>
       <c r="D74" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(B74="","-",IF(C74="","-",B74-C74))</f>
         <v>-</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B75">
-        <v>111196</v>
-      </c>
-      <c r="D75" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
+        <v>108885</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B76">
-        <v>111524</v>
+        <v>109301</v>
       </c>
       <c r="D76" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D76:D82" si="4">IF(B76="","-",IF(C76="","-",B76-C76))</f>
         <v>-</v>
       </c>
     </row>
@@ -1819,7 +1839,7 @@
         <v>68</v>
       </c>
       <c r="B77">
-        <v>112599</v>
+        <v>109728</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="4"/>
@@ -1831,7 +1851,7 @@
         <v>68</v>
       </c>
       <c r="B78">
-        <v>113555</v>
+        <v>111196</v>
       </c>
       <c r="D78" t="str">
         <f t="shared" si="4"/>
@@ -1840,10 +1860,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B79">
-        <v>117635</v>
+        <v>111524</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="4"/>
@@ -1852,63 +1872,63 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="B80">
+        <v>112599</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B81">
-        <v>121599</v>
+        <v>113555</v>
       </c>
       <c r="D81" t="str">
-        <f t="shared" ref="D81:D91" si="5">IF(B81="","-",IF(C81="","-",B81-C81))</f>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B82">
-        <v>126226</v>
+        <v>117635</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>75</v>
-      </c>
-      <c r="B83">
-        <v>136739</v>
-      </c>
-      <c r="D83" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B84">
-        <v>140173</v>
+        <v>121599</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D84:D94" si="5">IF(B84="","-",IF(C84="","-",B84-C84))</f>
         <v>-</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B85">
-        <v>141695</v>
+        <v>126226</v>
       </c>
       <c r="D85" t="str">
         <f t="shared" si="5"/>
@@ -1917,10 +1937,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="B86">
-        <v>146518</v>
+        <v>136739</v>
       </c>
       <c r="D86" t="str">
         <f t="shared" si="5"/>
@@ -1929,10 +1949,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B87">
-        <v>150651</v>
+        <v>140173</v>
       </c>
       <c r="D87" t="str">
         <f t="shared" si="5"/>
@@ -1941,10 +1961,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B88">
-        <v>156600</v>
+        <v>141695</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="5"/>
@@ -1953,10 +1973,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="B89">
-        <v>160147</v>
+        <v>146518</v>
       </c>
       <c r="D89" t="str">
         <f t="shared" si="5"/>
@@ -1965,10 +1985,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B90">
-        <v>175028</v>
+        <v>150651</v>
       </c>
       <c r="D90" t="str">
         <f t="shared" si="5"/>
@@ -1977,12 +1997,48 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91">
+        <v>156600</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>80</v>
+      </c>
+      <c r="B92">
+        <v>160147</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>81</v>
+      </c>
+      <c r="B93">
+        <v>175028</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>82</v>
       </c>
-      <c r="B91">
+      <c r="B94">
         <v>179257</v>
       </c>
-      <c r="D91" t="str">
+      <c r="D94" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
@@ -1997,7 +2053,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Super Tempo - level 4 done but wtih more points than idea, need to redo
</commit_message>
<xml_diff>
--- a/SuperTempo/SuperTempo-FC.xlsx
+++ b/SuperTempo/SuperTempo-FC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperTempo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EC2AB6-156E-4F96-9169-226B64471DF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EDE988-518F-400A-8771-4C438D4045E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41430" yWindow="2730" windowWidth="15870" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12630" yWindow="2730" windowWidth="15870" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="92">
   <si>
     <t>Place</t>
   </si>
@@ -374,6 +374,24 @@
   </si>
   <si>
     <t>hero appears</t>
+  </si>
+  <si>
+    <t>X = 101</t>
+  </si>
+  <si>
+    <t>X = 332</t>
+  </si>
+  <si>
+    <t>Hit count = 10</t>
+  </si>
+  <si>
+    <t>Hit count = 20</t>
+  </si>
+  <si>
+    <t>Hit count = 30</t>
+  </si>
+  <si>
+    <t>end countdown (score gone)</t>
   </si>
 </sst>
 </file>
@@ -766,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N94"/>
+  <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1431,7 +1449,7 @@
         <v>46725</v>
       </c>
       <c r="D44">
-        <f t="shared" ref="D44:D58" si="3">IF(B44="","-",IF(C44="","-",B44-C44))</f>
+        <f t="shared" ref="D44:D64" si="3">IF(B44="","-",IF(C44="","-",B44-C44))</f>
         <v>2435</v>
       </c>
     </row>
@@ -1491,7 +1509,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -1506,7 +1524,7 @@
         <v>4101</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1521,7 +1539,7 @@
         <v>4112</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>56</v>
       </c>
@@ -1536,7 +1554,7 @@
         <v>4263</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>84</v>
       </c>
@@ -1551,7 +1569,7 @@
         <v>4369</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -1566,7 +1584,7 @@
         <v>4369</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -1581,426 +1599,456 @@
         <v>4370</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55">
+        <v>68961</v>
+      </c>
+      <c r="C55">
+        <v>64591</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="3"/>
+        <v>4370</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56">
+        <v>69057</v>
+      </c>
+      <c r="C56">
+        <v>64687</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="3"/>
+        <v>4370</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57">
+        <v>69490</v>
+      </c>
+      <c r="C57">
+        <v>65111</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="3"/>
+        <v>4379</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58">
+        <v>70679</v>
+      </c>
+      <c r="C58">
+        <v>65921</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="3"/>
+        <v>4758</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59">
+        <v>71535</v>
+      </c>
+      <c r="C59">
+        <v>66752</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="3"/>
+        <v>4783</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>52</v>
       </c>
-      <c r="B55">
-        <v>74788</v>
-      </c>
-      <c r="D55" t="str">
+      <c r="B60">
+        <v>74787</v>
+      </c>
+      <c r="C60">
+        <v>69206</v>
+      </c>
+      <c r="D60">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+        <v>5581</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>53</v>
       </c>
-      <c r="B56">
+      <c r="B61">
         <v>75923</v>
       </c>
-      <c r="D56" t="str">
+      <c r="C61">
+        <v>70340</v>
+      </c>
+      <c r="D61">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+        <v>5583</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62">
+        <v>77087</v>
+      </c>
+      <c r="C62">
+        <v>71509</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="3"/>
+        <v>5578</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>54</v>
       </c>
-      <c r="B57">
+      <c r="B63">
         <v>78017</v>
       </c>
-      <c r="D57" t="str">
+      <c r="C63">
+        <v>72439</v>
+      </c>
+      <c r="D63">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+        <v>5578</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>12</v>
       </c>
-      <c r="B58">
+      <c r="B64">
         <v>79780</v>
       </c>
-      <c r="D58" t="str">
+      <c r="C64">
+        <v>74203</v>
+      </c>
+      <c r="D64">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+        <v>5577</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>12</v>
       </c>
-      <c r="B60">
+      <c r="B66">
         <v>79780</v>
-      </c>
-      <c r="D60" t="str">
-        <f>IF(B60="","-",IF(C60="","-",B60-C60))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>56</v>
-      </c>
-      <c r="B61">
-        <v>81636</v>
-      </c>
-      <c r="D61" t="str">
-        <f>IF(B61="","-",IF(C61="","-",B61-C61))</f>
-        <v>-</v>
-      </c>
-      <c r="E61" t="s">
-        <v>57</v>
-      </c>
-      <c r="F61" t="s">
-        <v>58</v>
-      </c>
-      <c r="G61" t="s">
-        <v>59</v>
-      </c>
-      <c r="H61" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62">
-        <v>82955</v>
-      </c>
-      <c r="D62" t="str">
-        <f>IF(B62="","-",IF(C62="","-",B62-C62))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>61</v>
-      </c>
-      <c r="B65">
-        <v>86049</v>
-      </c>
-      <c r="D65" t="str">
-        <f>IF(B65="","-",IF(C65="","-",B65-C65))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>63</v>
-      </c>
-      <c r="B66">
-        <v>87616</v>
       </c>
       <c r="D66" t="str">
         <f>IF(B66="","-",IF(C66="","-",B66-C66))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B67">
-        <v>89187</v>
+        <v>81636</v>
       </c>
       <c r="D67" t="str">
         <f>IF(B67="","-",IF(C67="","-",B67-C67))</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67" t="s">
+        <v>57</v>
+      </c>
+      <c r="F67" t="s">
+        <v>58</v>
+      </c>
+      <c r="G67" t="s">
+        <v>59</v>
+      </c>
+      <c r="H67" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B68">
-        <v>103048</v>
+        <v>82955</v>
       </c>
       <c r="D68" t="str">
         <f>IF(B68="","-",IF(C68="","-",B68-C68))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>66</v>
-      </c>
-      <c r="B69">
-        <v>106508</v>
-      </c>
-      <c r="D69" t="str">
-        <f>IF(B69="","-",IF(C69="","-",B69-C69))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B71">
-        <v>106508</v>
+        <v>86049</v>
       </c>
       <c r="D71" t="str">
         <f>IF(B71="","-",IF(C71="","-",B71-C71))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B72">
-        <v>107587</v>
+        <v>87616</v>
       </c>
       <c r="D72" t="str">
         <f>IF(B72="","-",IF(C72="","-",B72-C72))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B73">
-        <v>108015</v>
+        <v>89187</v>
       </c>
       <c r="D73" t="str">
         <f>IF(B73="","-",IF(C73="","-",B73-C73))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B74">
-        <v>108724</v>
+        <v>103048</v>
       </c>
       <c r="D74" t="str">
         <f>IF(B74="","-",IF(C74="","-",B74-C74))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B75">
-        <v>108885</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>68</v>
-      </c>
-      <c r="B76">
-        <v>109301</v>
-      </c>
-      <c r="D76" t="str">
-        <f t="shared" ref="D76:D82" si="4">IF(B76="","-",IF(C76="","-",B76-C76))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+        <v>106508</v>
+      </c>
+      <c r="D75" t="str">
+        <f>IF(B75="","-",IF(C75="","-",B75-C75))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B77">
-        <v>109728</v>
+        <v>106508</v>
       </c>
       <c r="D77" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+        <f>IF(B77="","-",IF(C77="","-",B77-C77))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>68</v>
       </c>
       <c r="B78">
-        <v>111196</v>
+        <v>107587</v>
       </c>
       <c r="D78" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+        <f>IF(B78="","-",IF(C78="","-",B78-C78))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B79">
-        <v>111524</v>
+        <v>108015</v>
       </c>
       <c r="D79" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+        <f>IF(B79="","-",IF(C79="","-",B79-C79))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B80">
-        <v>112599</v>
+        <v>108724</v>
       </c>
       <c r="D80" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(B80="","-",IF(C80="","-",B80-C80))</f>
         <v>-</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B81">
-        <v>113555</v>
-      </c>
-      <c r="D81" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
+        <v>108885</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B82">
-        <v>117635</v>
+        <v>109301</v>
       </c>
       <c r="D82" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="D82:D88" si="4">IF(B82="","-",IF(C82="","-",B82-C82))</f>
         <v>-</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="B83">
+        <v>109728</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B84">
-        <v>121599</v>
+        <v>111196</v>
       </c>
       <c r="D84" t="str">
-        <f t="shared" ref="D84:D94" si="5">IF(B84="","-",IF(C84="","-",B84-C84))</f>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B85">
-        <v>126226</v>
+        <v>111524</v>
       </c>
       <c r="D85" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B86">
-        <v>136739</v>
+        <v>112599</v>
       </c>
       <c r="D86" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B87">
-        <v>140173</v>
+        <v>113555</v>
       </c>
       <c r="D87" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B88">
-        <v>141695</v>
+        <v>117635</v>
       </c>
       <c r="D88" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>52</v>
-      </c>
-      <c r="B89">
-        <v>146518</v>
-      </c>
-      <c r="D89" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B90">
-        <v>150651</v>
+        <v>121599</v>
       </c>
       <c r="D90" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D90:D100" si="5">IF(B90="","-",IF(C90="","-",B90-C90))</f>
         <v>-</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B91">
-        <v>156600</v>
+        <v>126226</v>
       </c>
       <c r="D91" t="str">
         <f t="shared" si="5"/>
@@ -2009,10 +2057,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B92">
-        <v>160147</v>
+        <v>136739</v>
       </c>
       <c r="D92" t="str">
         <f t="shared" si="5"/>
@@ -2021,10 +2069,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B93">
-        <v>175028</v>
+        <v>140173</v>
       </c>
       <c r="D93" t="str">
         <f t="shared" si="5"/>
@@ -2033,12 +2081,84 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>77</v>
+      </c>
+      <c r="B94">
+        <v>141695</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>52</v>
+      </c>
+      <c r="B95">
+        <v>146518</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>78</v>
+      </c>
+      <c r="B96">
+        <v>150651</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>79</v>
+      </c>
+      <c r="B97">
+        <v>156600</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>80</v>
+      </c>
+      <c r="B98">
+        <v>160147</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>81</v>
+      </c>
+      <c r="B99">
+        <v>175028</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>82</v>
       </c>
-      <c r="B94">
+      <c r="B100">
         <v>179257</v>
       </c>
-      <c r="D94" t="str">
+      <c r="D100" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>

</xml_diff>

<commit_message>
Super Tempo - redo lv 4
</commit_message>
<xml_diff>
--- a/SuperTempo/SuperTempo-FC.xlsx
+++ b/SuperTempo/SuperTempo-FC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperTempo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EDE988-518F-400A-8771-4C438D4045E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E6DBCA-4F5E-4C4C-8FE4-7F67DF309FF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12630" yWindow="2730" windowWidth="15870" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16770" yWindow="855" windowWidth="15855" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="110">
   <si>
     <t>Place</t>
   </si>
@@ -392,6 +392,60 @@
   </si>
   <si>
     <t>end countdown (score gone)</t>
+  </si>
+  <si>
+    <t>x = 1899</t>
+  </si>
+  <si>
+    <t>x = 1473</t>
+  </si>
+  <si>
+    <t>X = 1243</t>
+  </si>
+  <si>
+    <t>X = 1128</t>
+  </si>
+  <si>
+    <t>X = 976</t>
+  </si>
+  <si>
+    <t>X = 1126</t>
+  </si>
+  <si>
+    <t>X = 1300</t>
+  </si>
+  <si>
+    <t>X = 1304</t>
+  </si>
+  <si>
+    <t>heroine appears</t>
+  </si>
+  <si>
+    <t>X = 2001</t>
+  </si>
+  <si>
+    <t>X = 1650</t>
+  </si>
+  <si>
+    <t>X = 80</t>
+  </si>
+  <si>
+    <t>X = 90</t>
+  </si>
+  <si>
+    <t>Hit count = 1</t>
+  </si>
+  <si>
+    <t>X = 586</t>
+  </si>
+  <si>
+    <t>X = 754 (160)</t>
+  </si>
+  <si>
+    <t>Stop walking</t>
+  </si>
+  <si>
+    <t>X = 1020</t>
   </si>
 </sst>
 </file>
@@ -784,10 +838,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N100"/>
+  <dimension ref="A1:N120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87:XFD87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1449,7 +1503,7 @@
         <v>46725</v>
       </c>
       <c r="D44">
-        <f t="shared" ref="D44:D64" si="3">IF(B44="","-",IF(C44="","-",B44-C44))</f>
+        <f t="shared" ref="D44:D83" si="3">IF(B44="","-",IF(C44="","-",B44-C44))</f>
         <v>2435</v>
       </c>
     </row>
@@ -1509,7 +1563,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -1523,8 +1577,15 @@
         <f t="shared" si="3"/>
         <v>4101</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>57931</v>
+      </c>
+      <c r="F49">
+        <f>IF(C49="","-",IF(E49="","-",C49-E49))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1538,628 +1599,1033 @@
         <f t="shared" si="3"/>
         <v>4112</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F50" t="str">
+        <f t="shared" ref="F50:F83" si="4">IF(C50="","-",IF(E50="","-",C50-E50))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51">
+        <v>58897</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="E51">
+        <v>58882</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52">
+        <v>59086</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="E52">
+        <v>59071</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53">
+        <v>59206</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="E53">
+        <v>59190</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54">
+        <v>59252</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="E54">
+        <v>59237</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55">
+        <v>59340</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="E55">
+        <v>59322</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56">
+        <v>59407</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="E56">
+        <v>59389</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57">
+        <v>59484</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="E57">
+        <v>59466</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58">
+        <v>59573</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="E58">
+        <v>59553</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>56</v>
       </c>
-      <c r="B51">
+      <c r="B60">
         <v>63983</v>
       </c>
-      <c r="C51">
+      <c r="C60">
         <v>59720</v>
       </c>
-      <c r="D51">
+      <c r="D60">
         <f t="shared" si="3"/>
         <v>4263</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="E60">
+        <v>59699</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61">
+        <v>60240</v>
+      </c>
+      <c r="E61">
+        <v>60218</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62">
+        <v>60600</v>
+      </c>
+      <c r="E62">
+        <v>60572</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>101</v>
+      </c>
+      <c r="C63">
+        <v>60791</v>
+      </c>
+      <c r="E63">
+        <v>60763</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>84</v>
       </c>
-      <c r="B52">
+      <c r="B64">
         <v>66173</v>
       </c>
-      <c r="C52">
+      <c r="C64">
         <v>61804</v>
       </c>
-      <c r="D52">
+      <c r="D64">
         <f t="shared" si="3"/>
         <v>4369</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="E64">
+        <v>61775</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>18</v>
       </c>
-      <c r="B53">
+      <c r="B65">
         <v>68394</v>
       </c>
-      <c r="C53">
+      <c r="C65">
         <v>64025</v>
       </c>
-      <c r="D53">
+      <c r="D65">
         <f t="shared" si="3"/>
         <v>4369</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="E65">
+        <v>63996</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>85</v>
       </c>
-      <c r="B54">
+      <c r="B66">
         <v>68825</v>
       </c>
-      <c r="C54">
+      <c r="C66">
         <v>64455</v>
       </c>
-      <c r="D54">
+      <c r="D66">
         <f t="shared" si="3"/>
         <v>4370</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="E66">
+        <v>64426</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67">
+        <v>64547</v>
+      </c>
+      <c r="E67">
+        <v>64518</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>104</v>
+      </c>
+      <c r="C68">
+        <v>64585</v>
+      </c>
+      <c r="E68">
+        <v>64556</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>86</v>
       </c>
-      <c r="B55">
+      <c r="B69">
         <v>68961</v>
       </c>
-      <c r="C55">
+      <c r="C69">
         <v>64591</v>
       </c>
-      <c r="D55">
+      <c r="D69">
         <f t="shared" si="3"/>
         <v>4370</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="E69">
+        <v>64562</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>87</v>
       </c>
-      <c r="B56">
+      <c r="B70">
         <v>69057</v>
       </c>
-      <c r="C56">
+      <c r="C70">
         <v>64687</v>
       </c>
-      <c r="D56">
+      <c r="D70">
         <f t="shared" si="3"/>
         <v>4370</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="E70">
+        <v>64658</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>105</v>
+      </c>
+      <c r="C71">
+        <v>65007</v>
+      </c>
+      <c r="E71">
+        <v>65001</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>88</v>
       </c>
-      <c r="B57">
+      <c r="B72">
         <v>69490</v>
       </c>
-      <c r="C57">
+      <c r="C72">
         <v>65111</v>
       </c>
-      <c r="D57">
+      <c r="D72">
         <f t="shared" si="3"/>
         <v>4379</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="E72">
+        <v>65071</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>89</v>
       </c>
-      <c r="B58">
+      <c r="B73">
         <v>70679</v>
       </c>
-      <c r="C58">
+      <c r="C73">
         <v>65921</v>
       </c>
-      <c r="D58">
+      <c r="D73">
         <f t="shared" si="3"/>
         <v>4758</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="E73">
+        <v>65912</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>90</v>
       </c>
-      <c r="B59">
+      <c r="B74">
         <v>71535</v>
       </c>
-      <c r="C59">
+      <c r="C74">
         <v>66752</v>
       </c>
-      <c r="D59">
+      <c r="D74">
         <f t="shared" si="3"/>
         <v>4783</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="E74">
+        <v>66730</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75">
+        <v>68112</v>
+      </c>
+      <c r="E75">
+        <v>68090</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>107</v>
+      </c>
+      <c r="C76">
+        <v>68183</v>
+      </c>
+      <c r="E76">
+        <v>68161</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>108</v>
+      </c>
+      <c r="C77">
+        <v>68235</v>
+      </c>
+      <c r="E77">
+        <v>68214</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>109</v>
+      </c>
+      <c r="C78">
+        <v>68668</v>
+      </c>
+      <c r="E78">
+        <v>68645</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>52</v>
       </c>
-      <c r="B60">
+      <c r="B79">
         <v>74787</v>
       </c>
-      <c r="C60">
-        <v>69206</v>
-      </c>
-      <c r="D60">
+      <c r="C79">
+        <v>69203</v>
+      </c>
+      <c r="D79">
         <f t="shared" si="3"/>
-        <v>5581</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+        <v>5584</v>
+      </c>
+      <c r="E79">
+        <v>69185</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>53</v>
       </c>
-      <c r="B61">
+      <c r="B80">
         <v>75923</v>
       </c>
-      <c r="C61">
+      <c r="C80">
         <v>70340</v>
       </c>
-      <c r="D61">
+      <c r="D80">
         <f t="shared" si="3"/>
         <v>5583</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="F80" t="str">
+        <f t="shared" si="4"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>91</v>
       </c>
-      <c r="B62">
+      <c r="B81">
         <v>77087</v>
       </c>
-      <c r="C62">
+      <c r="C81">
         <v>71509</v>
       </c>
-      <c r="D62">
+      <c r="D81">
         <f t="shared" si="3"/>
         <v>5578</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="E81">
+        <v>71325</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="4"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>54</v>
       </c>
-      <c r="B63">
+      <c r="B82">
         <v>78017</v>
       </c>
-      <c r="C63">
+      <c r="C82">
         <v>72439</v>
       </c>
-      <c r="D63">
+      <c r="D82">
         <f t="shared" si="3"/>
         <v>5578</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="E82">
+        <v>72255</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="4"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>12</v>
       </c>
-      <c r="B64">
+      <c r="B83">
         <v>79780</v>
       </c>
-      <c r="C64">
+      <c r="C83">
         <v>74203</v>
       </c>
-      <c r="D64">
+      <c r="D83">
         <f t="shared" si="3"/>
         <v>5577</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+      <c r="E83">
+        <v>74018</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="4"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>12</v>
       </c>
-      <c r="B66">
+      <c r="B85">
         <v>79780</v>
       </c>
-      <c r="D66" t="str">
-        <f>IF(B66="","-",IF(C66="","-",B66-C66))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="C85">
+        <v>74018</v>
+      </c>
+      <c r="D85">
+        <f>IF(B85="","-",IF(C85="","-",B85-C85))</f>
+        <v>5762</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>56</v>
       </c>
-      <c r="B67">
+      <c r="B86">
         <v>81636</v>
       </c>
-      <c r="D67" t="str">
-        <f>IF(B67="","-",IF(C67="","-",B67-C67))</f>
-        <v>-</v>
-      </c>
-      <c r="E67" t="s">
+      <c r="D86" t="str">
+        <f>IF(B86="","-",IF(C86="","-",B86-C86))</f>
+        <v>-</v>
+      </c>
+      <c r="E86" t="s">
         <v>57</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F86" t="s">
         <v>58</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G86" t="s">
         <v>59</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H86" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="87" spans="1:8" ht="16.5" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>60</v>
       </c>
-      <c r="B68">
+      <c r="B88">
         <v>82955</v>
       </c>
-      <c r="D68" t="str">
-        <f>IF(B68="","-",IF(C68="","-",B68-C68))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="D88" t="str">
+        <f>IF(B88="","-",IF(C88="","-",B88-C88))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+    <row r="90" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A90" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>61</v>
       </c>
-      <c r="B71">
+      <c r="B91">
         <v>86049</v>
       </c>
-      <c r="D71" t="str">
-        <f>IF(B71="","-",IF(C71="","-",B71-C71))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="D91" t="str">
+        <f>IF(B91="","-",IF(C91="","-",B91-C91))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>63</v>
       </c>
-      <c r="B72">
+      <c r="B92">
         <v>87616</v>
       </c>
-      <c r="D72" t="str">
-        <f>IF(B72="","-",IF(C72="","-",B72-C72))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="D92" t="str">
+        <f>IF(B92="","-",IF(C92="","-",B92-C92))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>64</v>
       </c>
-      <c r="B73">
+      <c r="B93">
         <v>89187</v>
       </c>
-      <c r="D73" t="str">
-        <f>IF(B73="","-",IF(C73="","-",B73-C73))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="D93" t="str">
+        <f>IF(B93="","-",IF(C93="","-",B93-C93))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>65</v>
       </c>
-      <c r="B74">
+      <c r="B94">
         <v>103048</v>
       </c>
-      <c r="D74" t="str">
-        <f>IF(B74="","-",IF(C74="","-",B74-C74))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="D94" t="str">
+        <f>IF(B94="","-",IF(C94="","-",B94-C94))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>66</v>
       </c>
-      <c r="B75">
+      <c r="B95">
         <v>106508</v>
       </c>
-      <c r="D75" t="str">
-        <f>IF(B75="","-",IF(C75="","-",B75-C75))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+      <c r="D95" t="str">
+        <f>IF(B95="","-",IF(C95="","-",B95-C95))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>66</v>
-      </c>
-      <c r="B77">
-        <v>106508</v>
-      </c>
-      <c r="D77" t="str">
-        <f>IF(B77="","-",IF(C77="","-",B77-C77))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>68</v>
-      </c>
-      <c r="B78">
-        <v>107587</v>
-      </c>
-      <c r="D78" t="str">
-        <f>IF(B78="","-",IF(C78="","-",B78-C78))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>68</v>
-      </c>
-      <c r="B79">
-        <v>108015</v>
-      </c>
-      <c r="D79" t="str">
-        <f>IF(B79="","-",IF(C79="","-",B79-C79))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>69</v>
-      </c>
-      <c r="B80">
-        <v>108724</v>
-      </c>
-      <c r="D80" t="str">
-        <f>IF(B80="","-",IF(C80="","-",B80-C80))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>70</v>
-      </c>
-      <c r="B81">
-        <v>108885</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>68</v>
-      </c>
-      <c r="B82">
-        <v>109301</v>
-      </c>
-      <c r="D82" t="str">
-        <f t="shared" ref="D82:D88" si="4">IF(B82="","-",IF(C82="","-",B82-C82))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>68</v>
-      </c>
-      <c r="B83">
-        <v>109728</v>
-      </c>
-      <c r="D83" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>68</v>
-      </c>
-      <c r="B84">
-        <v>111196</v>
-      </c>
-      <c r="D84" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>71</v>
-      </c>
-      <c r="B85">
-        <v>111524</v>
-      </c>
-      <c r="D85" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>68</v>
-      </c>
-      <c r="B86">
-        <v>112599</v>
-      </c>
-      <c r="D86" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>68</v>
-      </c>
-      <c r="B87">
-        <v>113555</v>
-      </c>
-      <c r="D87" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>72</v>
-      </c>
-      <c r="B88">
-        <v>117635</v>
-      </c>
-      <c r="D88" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
-        <v>71</v>
-      </c>
-      <c r="B90">
-        <v>121599</v>
-      </c>
-      <c r="D90" t="str">
-        <f t="shared" ref="D90:D100" si="5">IF(B90="","-",IF(C90="","-",B90-C90))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>74</v>
-      </c>
-      <c r="B91">
-        <v>126226</v>
-      </c>
-      <c r="D91" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>75</v>
-      </c>
-      <c r="B92">
-        <v>136739</v>
-      </c>
-      <c r="D92" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>76</v>
-      </c>
-      <c r="B93">
-        <v>140173</v>
-      </c>
-      <c r="D93" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>77</v>
-      </c>
-      <c r="B94">
-        <v>141695</v>
-      </c>
-      <c r="D94" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>52</v>
-      </c>
-      <c r="B95">
-        <v>146518</v>
-      </c>
-      <c r="D95" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>78</v>
-      </c>
-      <c r="B96">
-        <v>150651</v>
-      </c>
-      <c r="D96" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B97">
-        <v>156600</v>
+        <v>106508</v>
       </c>
       <c r="D97" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(B97="","-",IF(C97="","-",B97-C97))</f>
         <v>-</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B98">
-        <v>160147</v>
+        <v>107587</v>
       </c>
       <c r="D98" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(B98="","-",IF(C98="","-",B98-C98))</f>
         <v>-</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B99">
-        <v>175028</v>
+        <v>108015</v>
       </c>
       <c r="D99" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(B99="","-",IF(C99="","-",B99-C99))</f>
         <v>-</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>69</v>
+      </c>
+      <c r="B100">
+        <v>108724</v>
+      </c>
+      <c r="D100" t="str">
+        <f>IF(B100="","-",IF(C100="","-",B100-C100))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>70</v>
+      </c>
+      <c r="B101">
+        <v>108885</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>68</v>
+      </c>
+      <c r="B102">
+        <v>109301</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" ref="D102:D108" si="5">IF(B102="","-",IF(C102="","-",B102-C102))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>68</v>
+      </c>
+      <c r="B103">
+        <v>109728</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>68</v>
+      </c>
+      <c r="B104">
+        <v>111196</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>71</v>
+      </c>
+      <c r="B105">
+        <v>111524</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>68</v>
+      </c>
+      <c r="B106">
+        <v>112599</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>68</v>
+      </c>
+      <c r="B107">
+        <v>113555</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>72</v>
+      </c>
+      <c r="B108">
+        <v>117635</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>71</v>
+      </c>
+      <c r="B110">
+        <v>121599</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" ref="D110:D120" si="6">IF(B110="","-",IF(C110="","-",B110-C110))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>74</v>
+      </c>
+      <c r="B111">
+        <v>126226</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>75</v>
+      </c>
+      <c r="B112">
+        <v>136739</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>76</v>
+      </c>
+      <c r="B113">
+        <v>140173</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>77</v>
+      </c>
+      <c r="B114">
+        <v>141695</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>52</v>
+      </c>
+      <c r="B115">
+        <v>146518</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>78</v>
+      </c>
+      <c r="B116">
+        <v>150651</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>79</v>
+      </c>
+      <c r="B117">
+        <v>156600</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>80</v>
+      </c>
+      <c r="B118">
+        <v>160147</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>81</v>
+      </c>
+      <c r="B119">
+        <v>175028</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>82</v>
       </c>
-      <c r="B100">
+      <c r="B120">
         <v>179257</v>
       </c>
-      <c r="D100" t="str">
-        <f t="shared" si="5"/>
+      <c r="D120" t="str">
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first draft of lv 5 up to tower entrance
</commit_message>
<xml_diff>
--- a/SuperTempo/SuperTempo-FC.xlsx
+++ b/SuperTempo/SuperTempo-FC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperTempo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E6DBCA-4F5E-4C4C-8FE4-7F67DF309FF7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED87B3C0-F00A-4289-9A5A-C32007E8012F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16770" yWindow="855" windowWidth="15855" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="112">
   <si>
     <t>Place</t>
   </si>
@@ -446,6 +446,12 @@
   </si>
   <si>
     <t>X = 1020</t>
+  </si>
+  <si>
+    <t>Begin enter ship</t>
+  </si>
+  <si>
+    <t>First hop</t>
   </si>
 </sst>
 </file>
@@ -838,10 +844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N120"/>
+  <dimension ref="A1:N123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87:XFD87"/>
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2234,62 +2240,67 @@
         <v>5762</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="B86">
-        <v>81636</v>
-      </c>
-      <c r="D86" t="str">
+        <v>79861</v>
+      </c>
+      <c r="C86">
+        <v>74099</v>
+      </c>
+      <c r="D86">
         <f>IF(B86="","-",IF(C86="","-",B86-C86))</f>
-        <v>-</v>
-      </c>
-      <c r="E86" t="s">
-        <v>57</v>
-      </c>
-      <c r="F86" t="s">
-        <v>58</v>
-      </c>
-      <c r="G86" t="s">
-        <v>59</v>
-      </c>
-      <c r="H86" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="16.5" x14ac:dyDescent="0.2"/>
+        <v>5762</v>
+      </c>
+    </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="B88">
-        <v>82955</v>
-      </c>
-      <c r="D88" t="str">
+        <v>81493</v>
+      </c>
+      <c r="C88">
+        <v>75547</v>
+      </c>
+      <c r="D88">
         <f>IF(B88="","-",IF(C88="","-",B88-C88))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5946</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-    </row>
+        <v>56</v>
+      </c>
+      <c r="B89">
+        <v>81636</v>
+      </c>
+      <c r="D89" t="str">
+        <f>IF(B89="","-",IF(C89="","-",B89-C89))</f>
+        <v>-</v>
+      </c>
+      <c r="E89" t="s">
+        <v>57</v>
+      </c>
+      <c r="F89" t="s">
+        <v>58</v>
+      </c>
+      <c r="G89" t="s">
+        <v>59</v>
+      </c>
+      <c r="H89" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="16.5" x14ac:dyDescent="0.2"/>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B91">
-        <v>86049</v>
+        <v>82955</v>
       </c>
       <c r="D91" t="str">
         <f>IF(B91="","-",IF(C91="","-",B91-C91))</f>
@@ -2298,34 +2309,23 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>63</v>
-      </c>
-      <c r="B92">
-        <v>87616</v>
-      </c>
-      <c r="D92" t="str">
-        <f>IF(B92="","-",IF(C92="","-",B92-C92))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>64</v>
-      </c>
-      <c r="B93">
-        <v>89187</v>
-      </c>
-      <c r="D93" t="str">
-        <f>IF(B93="","-",IF(C93="","-",B93-C93))</f>
-        <v>-</v>
-      </c>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B94">
-        <v>103048</v>
+        <v>86049</v>
       </c>
       <c r="D94" t="str">
         <f>IF(B94="","-",IF(C94="","-",B94-C94))</f>
@@ -2334,30 +2334,34 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B95">
-        <v>106508</v>
+        <v>87616</v>
       </c>
       <c r="D95" t="str">
         <f>IF(B95="","-",IF(C95="","-",B95-C95))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>64</v>
+      </c>
+      <c r="B96">
+        <v>89187</v>
+      </c>
+      <c r="D96" t="str">
+        <f>IF(B96="","-",IF(C96="","-",B96-C96))</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B97">
-        <v>106508</v>
+        <v>103048</v>
       </c>
       <c r="D97" t="str">
         <f>IF(B97="","-",IF(C97="","-",B97-C97))</f>
@@ -2366,34 +2370,30 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B98">
-        <v>107587</v>
+        <v>106508</v>
       </c>
       <c r="D98" t="str">
         <f>IF(B98="","-",IF(C98="","-",B98-C98))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
-        <v>68</v>
-      </c>
-      <c r="B99">
-        <v>108015</v>
-      </c>
-      <c r="D99" t="str">
-        <f>IF(B99="","-",IF(C99="","-",B99-C99))</f>
-        <v>-</v>
-      </c>
+    <row r="99" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+      <c r="D99" s="1"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B100">
-        <v>108724</v>
+        <v>106508</v>
       </c>
       <c r="D100" t="str">
         <f>IF(B100="","-",IF(C100="","-",B100-C100))</f>
@@ -2402,10 +2402,14 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B101">
-        <v>108885</v>
+        <v>107587</v>
+      </c>
+      <c r="D101" t="str">
+        <f>IF(B101="","-",IF(C101="","-",B101-C101))</f>
+        <v>-</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -2413,46 +2417,42 @@
         <v>68</v>
       </c>
       <c r="B102">
-        <v>109301</v>
+        <v>108015</v>
       </c>
       <c r="D102" t="str">
-        <f t="shared" ref="D102:D108" si="5">IF(B102="","-",IF(C102="","-",B102-C102))</f>
+        <f>IF(B102="","-",IF(C102="","-",B102-C102))</f>
         <v>-</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B103">
-        <v>109728</v>
+        <v>108724</v>
       </c>
       <c r="D103" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(B103="","-",IF(C103="","-",B103-C103))</f>
         <v>-</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B104">
-        <v>111196</v>
-      </c>
-      <c r="D104" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
+        <v>108885</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B105">
-        <v>111524</v>
+        <v>109301</v>
       </c>
       <c r="D105" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="D105:D111" si="5">IF(B105="","-",IF(C105="","-",B105-C105))</f>
         <v>-</v>
       </c>
     </row>
@@ -2461,7 +2461,7 @@
         <v>68</v>
       </c>
       <c r="B106">
-        <v>112599</v>
+        <v>109728</v>
       </c>
       <c r="D106" t="str">
         <f t="shared" si="5"/>
@@ -2473,7 +2473,7 @@
         <v>68</v>
       </c>
       <c r="B107">
-        <v>113555</v>
+        <v>111196</v>
       </c>
       <c r="D107" t="str">
         <f t="shared" si="5"/>
@@ -2482,10 +2482,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B108">
-        <v>117635</v>
+        <v>111524</v>
       </c>
       <c r="D108" t="str">
         <f t="shared" si="5"/>
@@ -2494,63 +2494,63 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="B109">
+        <v>112599</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B110">
-        <v>121599</v>
+        <v>113555</v>
       </c>
       <c r="D110" t="str">
-        <f t="shared" ref="D110:D120" si="6">IF(B110="","-",IF(C110="","-",B110-C110))</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B111">
-        <v>126226</v>
+        <v>117635</v>
       </c>
       <c r="D111" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>75</v>
-      </c>
-      <c r="B112">
-        <v>136739</v>
-      </c>
-      <c r="D112" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
+        <v>73</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B113">
-        <v>140173</v>
+        <v>121599</v>
       </c>
       <c r="D113" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D113:D123" si="6">IF(B113="","-",IF(C113="","-",B113-C113))</f>
         <v>-</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B114">
-        <v>141695</v>
+        <v>126226</v>
       </c>
       <c r="D114" t="str">
         <f t="shared" si="6"/>
@@ -2559,10 +2559,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="B115">
-        <v>146518</v>
+        <v>136739</v>
       </c>
       <c r="D115" t="str">
         <f t="shared" si="6"/>
@@ -2571,10 +2571,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B116">
-        <v>150651</v>
+        <v>140173</v>
       </c>
       <c r="D116" t="str">
         <f t="shared" si="6"/>
@@ -2583,10 +2583,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B117">
-        <v>156600</v>
+        <v>141695</v>
       </c>
       <c r="D117" t="str">
         <f t="shared" si="6"/>
@@ -2595,10 +2595,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="B118">
-        <v>160147</v>
+        <v>146518</v>
       </c>
       <c r="D118" t="str">
         <f t="shared" si="6"/>
@@ -2607,10 +2607,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B119">
-        <v>175028</v>
+        <v>150651</v>
       </c>
       <c r="D119" t="str">
         <f t="shared" si="6"/>
@@ -2619,12 +2619,48 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
+        <v>79</v>
+      </c>
+      <c r="B120">
+        <v>156600</v>
+      </c>
+      <c r="D120" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>80</v>
+      </c>
+      <c r="B121">
+        <v>160147</v>
+      </c>
+      <c r="D121" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>81</v>
+      </c>
+      <c r="B122">
+        <v>175028</v>
+      </c>
+      <c r="D122" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
         <v>82</v>
       </c>
-      <c r="B120">
+      <c r="B123">
         <v>179257</v>
       </c>
-      <c r="D120" t="str">
+      <c r="D123" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>

</xml_diff>

<commit_message>
ST - up to level 7
</commit_message>
<xml_diff>
--- a/SuperTempo/SuperTempo-FC.xlsx
+++ b/SuperTempo/SuperTempo-FC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperTempo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED87B3C0-F00A-4289-9A5A-C32007E8012F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB219530-3CF9-4369-B332-CBBF42766EC0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16770" yWindow="855" windowWidth="15855" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16755" yWindow="855" windowWidth="15840" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="119">
   <si>
     <t>Place</t>
   </si>
@@ -452,6 +452,27 @@
   </si>
   <si>
     <t>First hop</t>
+  </si>
+  <si>
+    <t>Y = 800</t>
+  </si>
+  <si>
+    <t>q3 appears</t>
+  </si>
+  <si>
+    <t>q4 appears</t>
+  </si>
+  <si>
+    <t>q5 appears</t>
+  </si>
+  <si>
+    <t>begin exit</t>
+  </si>
+  <si>
+    <t>black screen</t>
+  </si>
+  <si>
+    <t>bonus screen end</t>
   </si>
 </sst>
 </file>
@@ -844,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N123"/>
+  <dimension ref="A1:N132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2270,238 +2291,262 @@
         <v>5946</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="16.5" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>56</v>
       </c>
-      <c r="B89">
+      <c r="B91">
         <v>81636</v>
-      </c>
-      <c r="D89" t="str">
-        <f>IF(B89="","-",IF(C89="","-",B89-C89))</f>
-        <v>-</v>
-      </c>
-      <c r="E89" t="s">
-        <v>57</v>
-      </c>
-      <c r="F89" t="s">
-        <v>58</v>
-      </c>
-      <c r="G89" t="s">
-        <v>59</v>
-      </c>
-      <c r="H89" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="16.5" x14ac:dyDescent="0.2"/>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>60</v>
-      </c>
-      <c r="B91">
-        <v>82955</v>
       </c>
       <c r="D91" t="str">
         <f>IF(B91="","-",IF(C91="","-",B91-C91))</f>
         <v>-</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
+      <c r="E91" t="s">
+        <v>57</v>
+      </c>
+      <c r="F91" t="s">
+        <v>58</v>
+      </c>
+      <c r="G91" t="s">
+        <v>59</v>
+      </c>
+      <c r="H91" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="16.5" x14ac:dyDescent="0.2"/>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>60</v>
+      </c>
+      <c r="B93">
+        <v>82955</v>
+      </c>
+      <c r="D93" t="str">
+        <f>IF(B93="","-",IF(C93="","-",B93-C93))</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>61</v>
       </c>
       <c r="B94">
-        <v>86049</v>
-      </c>
-      <c r="D94" t="str">
+        <v>83730</v>
+      </c>
+      <c r="C94">
+        <v>77216</v>
+      </c>
+      <c r="D94">
         <f>IF(B94="","-",IF(C94="","-",B94-C94))</f>
-        <v>-</v>
+        <v>6514</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B95">
-        <v>87616</v>
-      </c>
-      <c r="D95" t="str">
-        <f>IF(B95="","-",IF(C95="","-",B95-C95))</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>64</v>
-      </c>
-      <c r="B96">
-        <v>89187</v>
-      </c>
-      <c r="D96" t="str">
-        <f>IF(B96="","-",IF(C96="","-",B96-C96))</f>
-        <v>-</v>
-      </c>
+        <v>86049</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+      <c r="D96" s="1"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B97">
-        <v>103048</v>
-      </c>
-      <c r="D97" t="str">
+        <v>86049</v>
+      </c>
+      <c r="C97">
+        <v>79536</v>
+      </c>
+      <c r="D97">
         <f>IF(B97="","-",IF(C97="","-",B97-C97))</f>
-        <v>-</v>
+        <v>6513</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B98">
-        <v>106508</v>
+        <v>87616</v>
       </c>
       <c r="D98" t="str">
         <f>IF(B98="","-",IF(C98="","-",B98-C98))</f>
         <v>-</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>64</v>
+      </c>
+      <c r="B99">
+        <v>89186</v>
+      </c>
+      <c r="C99">
+        <v>82673</v>
+      </c>
+      <c r="D99">
+        <f>IF(B99="","-",IF(C99="","-",B99-C99))</f>
+        <v>6513</v>
+      </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>66</v>
+        <v>113</v>
       </c>
       <c r="B100">
-        <v>106508</v>
-      </c>
-      <c r="D100" t="str">
+        <v>92818</v>
+      </c>
+      <c r="C100">
+        <v>86305</v>
+      </c>
+      <c r="D100">
         <f>IF(B100="","-",IF(C100="","-",B100-C100))</f>
-        <v>-</v>
+        <v>6513</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
       <c r="B101">
-        <v>107587</v>
-      </c>
-      <c r="D101" t="str">
+        <v>94242</v>
+      </c>
+      <c r="C101">
+        <v>87729</v>
+      </c>
+      <c r="D101">
         <f>IF(B101="","-",IF(C101="","-",B101-C101))</f>
-        <v>-</v>
+        <v>6513</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>68</v>
+        <v>115</v>
       </c>
       <c r="B102">
-        <v>108015</v>
-      </c>
-      <c r="D102" t="str">
+        <v>95650</v>
+      </c>
+      <c r="C102">
+        <v>89137</v>
+      </c>
+      <c r="D102">
         <f>IF(B102="","-",IF(C102="","-",B102-C102))</f>
-        <v>-</v>
+        <v>6513</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="B103">
-        <v>108724</v>
-      </c>
-      <c r="D103" t="str">
+        <v>101844</v>
+      </c>
+      <c r="C103">
+        <v>95331</v>
+      </c>
+      <c r="D103">
         <f>IF(B103="","-",IF(C103="","-",B103-C103))</f>
-        <v>-</v>
+        <v>6513</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B104">
-        <v>108885</v>
+        <v>102561</v>
+      </c>
+      <c r="C104">
+        <v>96048</v>
+      </c>
+      <c r="D104">
+        <f>IF(B104="","-",IF(C104="","-",B104-C104))</f>
+        <v>6513</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="B105">
-        <v>109301</v>
-      </c>
-      <c r="D105" t="str">
-        <f t="shared" ref="D105:D111" si="5">IF(B105="","-",IF(C105="","-",B105-C105))</f>
-        <v>-</v>
+        <v>103048</v>
+      </c>
+      <c r="C105">
+        <v>96535</v>
+      </c>
+      <c r="D105">
+        <f>IF(B105="","-",IF(C105="","-",B105-C105))</f>
+        <v>6513</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="B106">
-        <v>109728</v>
-      </c>
-      <c r="D106" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
+        <v>105199</v>
+      </c>
+      <c r="C106">
+        <v>98049</v>
+      </c>
+      <c r="D106">
+        <f>IF(B106="","-",IF(C106="","-",B106-C106))</f>
+        <v>7150</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B107">
-        <v>111196</v>
-      </c>
-      <c r="D107" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>71</v>
-      </c>
-      <c r="B108">
-        <v>111524</v>
-      </c>
-      <c r="D108" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
+        <v>106508</v>
+      </c>
+      <c r="C107">
+        <v>99353</v>
+      </c>
+      <c r="D107">
+        <f>IF(B107="","-",IF(C107="","-",B107-C107))</f>
+        <v>7155</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B109">
-        <v>112599</v>
-      </c>
-      <c r="D109" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
+        <v>106508</v>
+      </c>
+      <c r="C109">
+        <v>99353</v>
+      </c>
+      <c r="D109">
+        <f>IF(B109="","-",IF(C109="","-",B109-C109))</f>
+        <v>7155</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -2509,158 +2554,262 @@
         <v>68</v>
       </c>
       <c r="B110">
-        <v>113555</v>
+        <v>107587</v>
       </c>
       <c r="D110" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(B110="","-",IF(C110="","-",B110-C110))</f>
         <v>-</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B111">
-        <v>117635</v>
+        <v>108015</v>
       </c>
       <c r="D111" t="str">
-        <f t="shared" si="5"/>
+        <f>IF(B111="","-",IF(C111="","-",B111-C111))</f>
         <v>-</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>73</v>
+        <v>69</v>
+      </c>
+      <c r="B112">
+        <v>108724</v>
+      </c>
+      <c r="D112" t="str">
+        <f>IF(B112="","-",IF(C112="","-",B112-C112))</f>
+        <v>-</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B113">
-        <v>121599</v>
-      </c>
-      <c r="D113" t="str">
-        <f t="shared" ref="D113:D123" si="6">IF(B113="","-",IF(C113="","-",B113-C113))</f>
-        <v>-</v>
+        <v>108885</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B114">
-        <v>126226</v>
+        <v>109301</v>
       </c>
       <c r="D114" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D114:D120" si="5">IF(B114="","-",IF(C114="","-",B114-C114))</f>
         <v>-</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B115">
-        <v>136739</v>
+        <v>109728</v>
       </c>
       <c r="D115" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B116">
-        <v>140173</v>
+        <v>111196</v>
       </c>
       <c r="D116" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B117">
-        <v>141695</v>
+        <v>111524</v>
       </c>
       <c r="D117" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B118">
-        <v>146518</v>
+        <v>112599</v>
       </c>
       <c r="D118" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B119">
-        <v>150651</v>
+        <v>113555</v>
       </c>
       <c r="D119" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B120">
-        <v>156600</v>
+        <v>117635</v>
       </c>
       <c r="D120" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>80</v>
-      </c>
-      <c r="B121">
-        <v>160147</v>
-      </c>
-      <c r="D121" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
+        <v>73</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B122">
-        <v>175028</v>
+        <v>121599</v>
       </c>
       <c r="D122" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="D122:D132" si="6">IF(B122="","-",IF(C122="","-",B122-C122))</f>
         <v>-</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>74</v>
+      </c>
+      <c r="B123">
+        <v>126226</v>
+      </c>
+      <c r="D123" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>75</v>
+      </c>
+      <c r="B124">
+        <v>136739</v>
+      </c>
+      <c r="D124" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>76</v>
+      </c>
+      <c r="B125">
+        <v>140173</v>
+      </c>
+      <c r="D125" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>77</v>
+      </c>
+      <c r="B126">
+        <v>141695</v>
+      </c>
+      <c r="D126" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>52</v>
+      </c>
+      <c r="B127">
+        <v>146518</v>
+      </c>
+      <c r="D127" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>78</v>
+      </c>
+      <c r="B128">
+        <v>150651</v>
+      </c>
+      <c r="D128" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>79</v>
+      </c>
+      <c r="B129">
+        <v>156600</v>
+      </c>
+      <c r="D129" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>80</v>
+      </c>
+      <c r="B130">
+        <v>160147</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>81</v>
+      </c>
+      <c r="B131">
+        <v>175028</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>82</v>
       </c>
-      <c r="B123">
+      <c r="B132">
         <v>179257</v>
       </c>
-      <c r="D123" t="str">
+      <c r="D132" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>

</xml_diff>

<commit_message>
ST - another boss fight done
</commit_message>
<xml_diff>
--- a/SuperTempo/SuperTempo-FC.xlsx
+++ b/SuperTempo/SuperTempo-FC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperTempo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B896070-D85E-4FC2-8F5A-BB722FDDEDAD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5850436-FCA3-4A77-9F0F-63F8C3B83B8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18960" yWindow="1140" windowWidth="15840" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="162">
   <si>
     <t>Place</t>
   </si>
@@ -578,6 +578,30 @@
   </si>
   <si>
     <t>Boss1HP = 0</t>
+  </si>
+  <si>
+    <t>Letter Get</t>
+  </si>
+  <si>
+    <t>Both Boss HP = 30</t>
+  </si>
+  <si>
+    <t>Both Boss HP = 20</t>
+  </si>
+  <si>
+    <t>Both Boss HP = 10</t>
+  </si>
+  <si>
+    <t>Both Boss HP = 0</t>
+  </si>
+  <si>
+    <t>Both Letter Get</t>
+  </si>
+  <si>
+    <t>Start run</t>
+  </si>
+  <si>
+    <t>Boss 3 appears</t>
   </si>
 </sst>
 </file>
@@ -970,10 +994,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N193"/>
+  <dimension ref="A1:N200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="A188" sqref="A188"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="C196" sqref="C196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3014,7 +3038,7 @@
         <v>114059</v>
       </c>
       <c r="D134">
-        <f t="shared" ref="D134:D193" si="7">IF(B134="","-",IF(C134="","-",B134-C134))</f>
+        <f t="shared" ref="D134:D200" si="7">IF(B134="","-",IF(C134="","-",B134-C134))</f>
         <v>7540</v>
       </c>
     </row>
@@ -3697,55 +3721,146 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D187" t="str">
+      <c r="A187" t="s">
+        <v>154</v>
+      </c>
+      <c r="B187">
+        <v>161921</v>
+      </c>
+      <c r="C187">
+        <v>150349</v>
+      </c>
+      <c r="D187">
+        <f t="shared" si="7"/>
+        <v>11572</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>155</v>
+      </c>
+      <c r="B188">
+        <v>162219</v>
+      </c>
+      <c r="C188">
+        <v>150691</v>
+      </c>
+      <c r="D188">
+        <f t="shared" si="7"/>
+        <v>11528</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>156</v>
+      </c>
+      <c r="B189">
+        <v>162499</v>
+      </c>
+      <c r="C189">
+        <v>150931</v>
+      </c>
+      <c r="D189">
+        <f t="shared" si="7"/>
+        <v>11568</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>157</v>
+      </c>
+      <c r="B190">
+        <v>162755</v>
+      </c>
+      <c r="D190" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D188" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D189" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D190" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
-    </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D191" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
+      <c r="A191" t="s">
+        <v>160</v>
+      </c>
+      <c r="C191">
+        <v>151267</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>81</v>
-      </c>
-      <c r="B192">
-        <v>175028</v>
-      </c>
-      <c r="D192" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
+        <v>160</v>
+      </c>
+      <c r="C192">
+        <v>151435</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>158</v>
+      </c>
+      <c r="B193">
+        <v>163167</v>
+      </c>
+      <c r="C193">
+        <v>151418</v>
+      </c>
+      <c r="D193">
+        <f t="shared" si="7"/>
+        <v>11749</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>159</v>
+      </c>
+      <c r="B194">
+        <v>163502</v>
+      </c>
+      <c r="D194" t="str">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>161</v>
+      </c>
+      <c r="B195">
+        <v>163623</v>
+      </c>
+      <c r="C195">
+        <v>151874</v>
+      </c>
+      <c r="D195">
+        <f t="shared" si="7"/>
+        <v>11749</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D198" t="str">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>81</v>
+      </c>
+      <c r="B199">
+        <v>175028</v>
+      </c>
+      <c r="D199" t="str">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
         <v>82</v>
       </c>
-      <c r="B193">
+      <c r="B200">
         <v>179257</v>
       </c>
-      <c r="D193" t="str">
+      <c r="D200" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>

</xml_diff>

<commit_message>
ST - up to final boss fight
</commit_message>
<xml_diff>
--- a/SuperTempo/SuperTempo-FC.xlsx
+++ b/SuperTempo/SuperTempo-FC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperTempo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5850436-FCA3-4A77-9F0F-63F8C3B83B8B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D42B03-FC9F-4B24-BE92-4A43184D348D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18960" yWindow="1140" windowWidth="15840" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="177">
   <si>
     <t>Place</t>
   </si>
@@ -602,6 +602,51 @@
   </si>
   <si>
     <t>Boss 3 appears</t>
+  </si>
+  <si>
+    <t>Boss 3 HP = 0</t>
+  </si>
+  <si>
+    <t>Boss 4 appears</t>
+  </si>
+  <si>
+    <t>Boss 4 HP = 40</t>
+  </si>
+  <si>
+    <t>Boss 4 HP = 30</t>
+  </si>
+  <si>
+    <t>Boss 4 HP = 20</t>
+  </si>
+  <si>
+    <t>Boss 4 HP = 10</t>
+  </si>
+  <si>
+    <t>Boss 4 HP = 0</t>
+  </si>
+  <si>
+    <t>Boss 5 appears</t>
+  </si>
+  <si>
+    <t>Boss 5 HP = 50</t>
+  </si>
+  <si>
+    <t>Boss 5 HP = 40</t>
+  </si>
+  <si>
+    <t>Boss 5 HP = 30</t>
+  </si>
+  <si>
+    <t>Boss 5 HP = 20</t>
+  </si>
+  <si>
+    <t>Boss 5 HP = 10</t>
+  </si>
+  <si>
+    <t>Boss 5 HP = 00</t>
+  </si>
+  <si>
+    <t>start fight</t>
   </si>
 </sst>
 </file>
@@ -994,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N200"/>
+  <dimension ref="A1:N216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="C196" sqref="C196"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="B214" sqref="B214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3038,7 +3083,7 @@
         <v>114059</v>
       </c>
       <c r="D134">
-        <f t="shared" ref="D134:D200" si="7">IF(B134="","-",IF(C134="","-",B134-C134))</f>
+        <f t="shared" ref="D134:D216" si="7">IF(B134="","-",IF(C134="","-",B134-C134))</f>
         <v>7540</v>
       </c>
     </row>
@@ -3835,32 +3880,259 @@
         <v>11749</v>
       </c>
     </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>162</v>
+      </c>
+      <c r="B197">
+        <v>165246</v>
+      </c>
+      <c r="C197">
+        <v>153517</v>
+      </c>
+      <c r="D197">
+        <f t="shared" si="7"/>
+        <v>11729</v>
+      </c>
+    </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D198" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
+      <c r="A198" t="s">
+        <v>163</v>
+      </c>
+      <c r="B198">
+        <v>165462</v>
+      </c>
+      <c r="C198">
+        <v>153699</v>
+      </c>
+      <c r="D198">
+        <f t="shared" si="7"/>
+        <v>11763</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
       <c r="B199">
-        <v>175028</v>
-      </c>
-      <c r="D199" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
+        <v>165547</v>
+      </c>
+      <c r="C199">
+        <v>153784</v>
+      </c>
+      <c r="D199">
+        <f t="shared" si="7"/>
+        <v>11763</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
+        <v>165</v>
+      </c>
+      <c r="B200">
+        <v>165788</v>
+      </c>
+      <c r="C200">
+        <v>154025</v>
+      </c>
+      <c r="D200">
+        <f t="shared" si="7"/>
+        <v>11763</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>166</v>
+      </c>
+      <c r="B201">
+        <v>166029</v>
+      </c>
+      <c r="C201">
+        <v>154266</v>
+      </c>
+      <c r="D201">
+        <f t="shared" si="7"/>
+        <v>11763</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>167</v>
+      </c>
+      <c r="B202">
+        <v>166282</v>
+      </c>
+      <c r="C202">
+        <v>154507</v>
+      </c>
+      <c r="D202">
+        <f t="shared" si="7"/>
+        <v>11775</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>168</v>
+      </c>
+      <c r="B203">
+        <v>166526</v>
+      </c>
+      <c r="C203">
+        <v>154747</v>
+      </c>
+      <c r="D203">
+        <f t="shared" si="7"/>
+        <v>11779</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>169</v>
+      </c>
+      <c r="B204">
+        <v>167321</v>
+      </c>
+      <c r="C204">
+        <v>155542</v>
+      </c>
+      <c r="D204">
+        <f t="shared" si="7"/>
+        <v>11779</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>170</v>
+      </c>
+      <c r="B205">
+        <v>167361</v>
+      </c>
+      <c r="C205">
+        <v>155582</v>
+      </c>
+      <c r="D205">
+        <f t="shared" si="7"/>
+        <v>11779</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>171</v>
+      </c>
+      <c r="B206">
+        <v>167603</v>
+      </c>
+      <c r="C206">
+        <v>155822</v>
+      </c>
+      <c r="D206">
+        <f t="shared" si="7"/>
+        <v>11781</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>172</v>
+      </c>
+      <c r="B207">
+        <v>167849</v>
+      </c>
+      <c r="C207">
+        <v>156062</v>
+      </c>
+      <c r="D207">
+        <f t="shared" si="7"/>
+        <v>11787</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>173</v>
+      </c>
+      <c r="B208">
+        <v>168155</v>
+      </c>
+      <c r="C208">
+        <v>156302</v>
+      </c>
+      <c r="D208">
+        <f t="shared" si="7"/>
+        <v>11853</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>174</v>
+      </c>
+      <c r="B209">
+        <v>168559</v>
+      </c>
+      <c r="C209">
+        <v>156542</v>
+      </c>
+      <c r="D209">
+        <f t="shared" si="7"/>
+        <v>12017</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>175</v>
+      </c>
+      <c r="B210">
+        <v>168967</v>
+      </c>
+      <c r="C210">
+        <v>156782</v>
+      </c>
+      <c r="D210">
+        <f t="shared" si="7"/>
+        <v>12185</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C211">
+        <v>157395</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>81</v>
+      </c>
+      <c r="B212">
+        <v>175028</v>
+      </c>
+      <c r="C212">
+        <v>162843</v>
+      </c>
+      <c r="D212">
+        <f t="shared" si="7"/>
+        <v>12185</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>176</v>
+      </c>
+      <c r="B213">
+        <v>175962</v>
+      </c>
+      <c r="C213">
+        <v>163774</v>
+      </c>
+      <c r="D213">
+        <f t="shared" si="7"/>
+        <v>12188</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
         <v>82</v>
       </c>
-      <c r="B200">
+      <c r="B216">
         <v>179257</v>
       </c>
-      <c r="D200" t="str">
+      <c r="D216" t="str">
         <f t="shared" si="7"/>
         <v>-</v>
       </c>

</xml_diff>

<commit_message>
ST - final boss done, first attempt
</commit_message>
<xml_diff>
--- a/SuperTempo/SuperTempo-FC.xlsx
+++ b/SuperTempo/SuperTempo-FC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\SuperTempo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D42B03-FC9F-4B24-BE92-4A43184D348D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A92AFE-EFFF-4775-8DEB-4FE4DD93A069}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18960" yWindow="1140" windowWidth="15840" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:N216"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+      <selection activeCell="C217" sqref="C217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4132,9 +4132,12 @@
       <c r="B216">
         <v>179257</v>
       </c>
-      <c r="D216" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
+      <c r="C216">
+        <v>165474</v>
+      </c>
+      <c r="D216">
+        <f t="shared" si="7"/>
+        <v>13783</v>
       </c>
     </row>
   </sheetData>

</xml_diff>